<commit_message>
* resolvido problema de exclusao de cartao (and pretty much delete eny other things from "list desp.xlsx" too...)
</commit_message>
<xml_diff>
--- a/listas desp.xlsx
+++ b/listas desp.xlsx
@@ -478,7 +478,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>tipo</t>
   </si>
@@ -3331,7 +3331,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="19.5">
@@ -3440,7 +3440,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="3" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="3" customWidth="true" width="19.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19.5">
@@ -3487,28 +3487,6 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="2">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="2">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>